<commit_message>
opt for stoplose and holiday
</commit_message>
<xml_diff>
--- a/Docs/report_abstract.xlsx
+++ b/Docs/report_abstract.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>EURUSD</t>
   </si>
@@ -161,10 +161,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>我choose</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -193,7 +189,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>注:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>USD,CAD经济体关系大，所以EURUSD与EURCAD共用仓位额度</t>
+  </si>
+  <si>
+    <t>非农数据公布天强制close会造成利润大幅减少，建议4H级别以上不强制close，只是不开新单</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beta</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -681,11 +688,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R24" sqref="R24"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -703,7 +710,7 @@
     <col min="11" max="11" width="9" style="3" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="3" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="8.25" style="3" hidden="1" customWidth="1"/>
-    <col min="14" max="17" width="9" style="2" hidden="1" customWidth="1"/>
+    <col min="14" max="17" width="9" style="2" customWidth="1"/>
     <col min="18" max="19" width="9" style="2"/>
     <col min="20" max="20" width="12.5" style="2" customWidth="1"/>
     <col min="21" max="16384" width="9" style="2"/>
@@ -750,25 +757,28 @@
         <v>33</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="5" t="s">
-        <v>48</v>
+      <c r="U1" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="15" customFormat="1">
@@ -832,8 +842,8 @@
       <c r="T2" s="15">
         <v>0.01</v>
       </c>
-      <c r="U2" s="15" t="s">
-        <v>49</v>
+      <c r="U2" s="15">
+        <v>622</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="19" customFormat="1">
@@ -938,6 +948,9 @@
       <c r="T4" s="17">
         <v>0.01</v>
       </c>
+      <c r="U4" s="17">
+        <v>655</v>
+      </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="2" t="s">
@@ -1118,6 +1131,9 @@
       <c r="T7" s="17">
         <v>0.01</v>
       </c>
+      <c r="U7" s="17">
+        <v>442</v>
+      </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="2" t="s">
@@ -1177,6 +1193,9 @@
       <c r="S9" s="2">
         <v>60</v>
       </c>
+      <c r="U9" s="2">
+        <v>-8</v>
+      </c>
     </row>
     <row r="10" spans="1:21" s="19" customFormat="1">
       <c r="A10" s="19" t="s">
@@ -1338,6 +1357,9 @@
       <c r="T13" s="17">
         <v>0.01</v>
       </c>
+      <c r="U13" s="17">
+        <v>603</v>
+      </c>
     </row>
     <row r="15" spans="1:21" s="23" customFormat="1">
       <c r="A15" s="23" t="s">
@@ -1445,7 +1467,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="19" customFormat="1">
+    <row r="17" spans="1:21" s="19" customFormat="1">
       <c r="A17" s="19" t="s">
         <v>13</v>
       </c>
@@ -1486,7 +1508,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="19" customFormat="1">
+    <row r="18" spans="1:21" s="19" customFormat="1">
       <c r="A18" s="19" t="s">
         <v>14</v>
       </c>
@@ -1494,7 +1516,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:21">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
@@ -1547,7 +1569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="23" customFormat="1">
+    <row r="21" spans="1:21" s="23" customFormat="1">
       <c r="A21" s="23" t="s">
         <v>16</v>
       </c>
@@ -1606,7 +1628,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="21" customFormat="1">
+    <row r="22" spans="1:21" s="21" customFormat="1">
       <c r="A22" s="21" t="s">
         <v>17</v>
       </c>
@@ -1667,8 +1689,11 @@
       <c r="T22" s="21">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" s="17" customFormat="1">
+      <c r="U22" s="21">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" s="17" customFormat="1">
       <c r="A24" s="17" t="s">
         <v>18</v>
       </c>
@@ -1715,13 +1740,13 @@
         <v>60</v>
       </c>
       <c r="P24" s="17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Q24" s="17">
         <v>70</v>
       </c>
       <c r="R24" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S24" s="17">
         <v>70</v>
@@ -1729,8 +1754,11 @@
       <c r="T24" s="17">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" s="19" customFormat="1">
+      <c r="U24" s="17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" s="19" customFormat="1">
       <c r="A25" s="19" t="s">
         <v>19</v>
       </c>
@@ -1771,7 +1799,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="19" customFormat="1">
+    <row r="26" spans="1:21" s="19" customFormat="1">
       <c r="A26" s="19" t="s">
         <v>20</v>
       </c>
@@ -1810,6 +1838,21 @@
       </c>
       <c r="M26" s="20">
         <v>0.83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>